<commit_message>
Add predict_proba method to RiskModelPipeline
</commit_message>
<xml_diff>
--- a/notebooks/pipeline_test_output/model_report.xlsx
+++ b/notebooks/pipeline_test_output/model_report.xlsx
@@ -1292,28 +1292,28 @@
         <v>25.81403155421282</v>
       </c>
       <c r="D6" t="n">
-        <v>6.048387096774194</v>
+        <v>24.05913978494624</v>
       </c>
       <c r="E6" t="n">
         <v>769</v>
       </c>
       <c r="F6" t="n">
-        <v>45</v>
+        <v>179</v>
       </c>
       <c r="G6" t="n">
-        <v>-19.76564445743863</v>
+        <v>-1.754891769266587</v>
       </c>
       <c r="H6" t="n">
-        <v>0.2868245168437391</v>
+        <v>0.0012355007655722</v>
       </c>
       <c r="I6" t="n">
         <v>0.2654176597601441</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2318704635091582</v>
+        <v>0.2653365456990043</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2910129013330919</v>
+        <v>0.005423885254925055</v>
       </c>
     </row>
     <row r="7">
@@ -1329,28 +1329,28 @@
         <v>3.759650889560255</v>
       </c>
       <c r="D7" t="n">
-        <v>22.58064516129032</v>
+        <v>4.56989247311828</v>
       </c>
       <c r="E7" t="n">
         <v>112</v>
       </c>
       <c r="F7" t="n">
-        <v>168</v>
+        <v>34</v>
       </c>
       <c r="G7" t="n">
-        <v>18.82099427173007</v>
+        <v>0.8102415835580246</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3374165792667337</v>
+        <v>0.00158129640982946</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3204213058735214</v>
+        <v>0.3204213058735216</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2845053176750524</v>
+        <v>0.315759486682328</v>
       </c>
       <c r="K7" t="n">
-        <v>0.6284294805998256</v>
+        <v>0.007005181664754515</v>
       </c>
     </row>
   </sheetData>
@@ -1460,7 +1460,7 @@
         <v>0.1414825556377363</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1416258266621569</v>
+        <v>0.1416258266621568</v>
       </c>
       <c r="K2" t="n">
         <v>0.0001132393323321938</v>
@@ -1479,28 +1479,28 @@
         <v>22.35649546827795</v>
       </c>
       <c r="D3" t="n">
-        <v>2.036021926389977</v>
+        <v>20.6734534064213</v>
       </c>
       <c r="E3" t="n">
         <v>666</v>
       </c>
       <c r="F3" t="n">
-        <v>26</v>
+        <v>264</v>
       </c>
       <c r="G3" t="n">
-        <v>-20.32047354188797</v>
+        <v>-1.683042061856646</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4869027347096352</v>
+        <v>0.001317257622436057</v>
       </c>
       <c r="I3" t="n">
         <v>0.1518364427420138</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1464245196322003</v>
+        <v>0.1520087400391462</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4870159740419674</v>
+        <v>0.001430496954768251</v>
       </c>
     </row>
     <row r="4">
@@ -1516,28 +1516,28 @@
         <v>23.69922792883518</v>
       </c>
       <c r="D4" t="n">
-        <v>24.58888018794049</v>
+        <v>24.66718872357087</v>
       </c>
       <c r="E4" t="n">
         <v>706</v>
       </c>
       <c r="F4" t="n">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8896522591053058</v>
+        <v>0.9679607947356894</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0003278532724163654</v>
+        <v>0.0003874892063125338</v>
       </c>
       <c r="I4" t="n">
         <v>0.1846848714523704</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1581405765688158</v>
+        <v>0.1842496862321489</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4873438273143837</v>
+        <v>0.001817986161080785</v>
       </c>
     </row>
     <row r="5">
@@ -1553,28 +1553,28 @@
         <v>3.289694528365223</v>
       </c>
       <c r="D5" t="n">
-        <v>21.1433046202036</v>
+        <v>3.680501174628034</v>
       </c>
       <c r="E5" t="n">
         <v>98</v>
       </c>
       <c r="F5" t="n">
-        <v>270</v>
+        <v>47</v>
       </c>
       <c r="G5" t="n">
-        <v>17.85361009183838</v>
+        <v>0.3908066462628111</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3321715177863347</v>
+        <v>0.0004386969513771168</v>
       </c>
       <c r="I5" t="n">
         <v>0.2006989914196349</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1884690140537783</v>
+        <v>0.20306586887407</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8195153451007184</v>
+        <v>0.002256683112457901</v>
       </c>
     </row>
     <row r="6">
@@ -1590,28 +1590,28 @@
         <v>25.81403155421282</v>
       </c>
       <c r="D6" t="n">
-        <v>27.79953014878622</v>
+        <v>26.54659357870008</v>
       </c>
       <c r="E6" t="n">
         <v>769</v>
       </c>
       <c r="F6" t="n">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="G6" t="n">
-        <v>1.985498594573393</v>
+        <v>0.7325620244872544</v>
       </c>
       <c r="H6" t="n">
-        <v>0.001471272658661972</v>
+        <v>0.0002049945495771488</v>
       </c>
       <c r="I6" t="n">
         <v>0.2654176597601441</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2638713708698848</v>
+        <v>0.266404408955256</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8209866177593804</v>
+        <v>0.00246167766203505</v>
       </c>
     </row>
     <row r="7">
@@ -1642,13 +1642,13 @@
         <v>1.579987286193194e-05</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3204213058735214</v>
+        <v>0.3204213058735216</v>
       </c>
       <c r="J7" t="n">
-        <v>0.3151734183105581</v>
+        <v>0.315173418310558</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8210024176322424</v>
+        <v>0.002477477534896982</v>
       </c>
     </row>
   </sheetData>
@@ -1817,7 +1817,7 @@
         <v>27.5</v>
       </c>
       <c r="F3" t="n">
-        <v>26.36360920517068</v>
+        <v>26.36360920517067</v>
       </c>
       <c r="G3" t="n">
         <v>18.58190709046455</v>
@@ -2012,7 +2012,7 @@
         <v>22.83464566929134</v>
       </c>
       <c r="G2" t="n">
-        <v>8.719101405670598</v>
+        <v>8.719101405670601</v>
       </c>
       <c r="H2" t="n">
         <v>16.39556223010246</v>
@@ -2026,7 +2026,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>0.007211321588540953</v>
+        <v>0.007211321588540948</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -2153,13 +2153,13 @@
         <v>30</v>
       </c>
       <c r="E5" t="n">
-        <v>15.26187809239384</v>
+        <v>15.26187809239385</v>
       </c>
       <c r="F5" t="n">
         <v>23.62204724409449</v>
       </c>
       <c r="G5" t="n">
-        <v>8.360169151700644</v>
+        <v>8.360169151700639</v>
       </c>
       <c r="H5" t="n">
         <v>17.07730427990417</v>
@@ -2173,7 +2173,7 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0.01299428876467781</v>
+        <v>0.01299428876467782</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Major refactor: Add UnifiedRiskPipeline V2 with complete features
- Single pipeline controlled by config (no more multiple pipeline classes)
- Scoring optional (default OFF)
- Data dictionary support for variable descriptions
- Stage 1 & Stage 2 calibration engine
- Separate numeric/categorical data handling
- Updated selection order: PSI->VIF->Correlation->IV->Boruta->Stepwise
- Univariate Gini calculation for all features
- Comprehensive refactor plan documented
</commit_message>
<xml_diff>
--- a/notebooks/pipeline_test_output/model_report.xlsx
+++ b/notebooks/pipeline_test_output/model_report.xlsx
@@ -1310,7 +1310,7 @@
         <v>0.2654176597601441</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2653365456990043</v>
+        <v>0.2653365456990042</v>
       </c>
       <c r="K6" t="n">
         <v>0.005423885254925055</v>
@@ -1460,7 +1460,7 @@
         <v>0.1414825556377363</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1416258266621568</v>
+        <v>0.1416258266621569</v>
       </c>
       <c r="K2" t="n">
         <v>0.0001132393323321938</v>
@@ -1817,7 +1817,7 @@
         <v>27.5</v>
       </c>
       <c r="F3" t="n">
-        <v>26.36360920517067</v>
+        <v>26.36360920517068</v>
       </c>
       <c r="G3" t="n">
         <v>18.58190709046455</v>
@@ -2110,7 +2110,7 @@
         <v>22.83464566929134</v>
       </c>
       <c r="G4" t="n">
-        <v>7.774369215401119</v>
+        <v>7.774369215401114</v>
       </c>
       <c r="H4" t="n">
         <v>16.39556223010246</v>
@@ -2124,7 +2124,7 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>0.01817058965418702</v>
+        <v>0.01817058965418706</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -2159,7 +2159,7 @@
         <v>23.62204724409449</v>
       </c>
       <c r="G5" t="n">
-        <v>8.360169151700639</v>
+        <v>8.360169151700635</v>
       </c>
       <c r="H5" t="n">
         <v>17.07730427990417</v>
@@ -2173,7 +2173,7 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0.01299428876467782</v>
+        <v>0.01299428876467788</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -2398,7 +2398,7 @@
         <v>20</v>
       </c>
       <c r="E10" t="n">
-        <v>27.6575155389624</v>
+        <v>27.65751553896241</v>
       </c>
       <c r="F10" t="n">
         <v>15.74803149606299</v>
@@ -2418,7 +2418,7 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>0.00200951047228893</v>
+        <v>0.002009510472288933</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -2447,13 +2447,13 @@
         <v>34</v>
       </c>
       <c r="E11" t="n">
-        <v>29.06894455622044</v>
+        <v>29.06894455622045</v>
       </c>
       <c r="F11" t="n">
         <v>25.37313432835821</v>
       </c>
       <c r="G11" t="n">
-        <v>-3.695810227862228</v>
+        <v>-3.69581022786224</v>
       </c>
       <c r="H11" t="n">
         <v>18.76281924434715</v>
@@ -2467,7 +2467,7 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>0.3921068605837145</v>
+        <v>0.3921068605837161</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
chore(repo): include local notebooks, examples and new modules
</commit_message>
<xml_diff>
--- a/notebooks/pipeline_test_output/model_report.xlsx
+++ b/notebooks/pipeline_test_output/model_report.xlsx
@@ -1162,7 +1162,7 @@
         <v>0.1414825556377363</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1415682038751703</v>
+        <v>0.1415682038751702</v>
       </c>
       <c r="K2" t="n">
         <v>2.924533268114003e-05</v>
@@ -1497,7 +1497,7 @@
         <v>0.1518364427420138</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1520087400391462</v>
+        <v>0.1520087400391461</v>
       </c>
       <c r="K3" t="n">
         <v>0.001430496954768251</v>
@@ -1608,7 +1608,7 @@
         <v>0.2654176597601441</v>
       </c>
       <c r="J6" t="n">
-        <v>0.266404408955256</v>
+        <v>0.2664044089552561</v>
       </c>
       <c r="K6" t="n">
         <v>0.00246167766203505</v>
@@ -1763,7 +1763,7 @@
         <v>15</v>
       </c>
       <c r="F2" t="n">
-        <v>16.12582605077666</v>
+        <v>16.12582605077665</v>
       </c>
       <c r="G2" t="n">
         <v>19.81242672919109</v>
@@ -2006,13 +2006,13 @@
         <v>29</v>
       </c>
       <c r="E2" t="n">
-        <v>14.11554426362074</v>
+        <v>14.11554426362073</v>
       </c>
       <c r="F2" t="n">
         <v>22.83464566929134</v>
       </c>
       <c r="G2" t="n">
-        <v>8.719101405670601</v>
+        <v>8.71910140567061</v>
       </c>
       <c r="H2" t="n">
         <v>16.39556223010246</v>
@@ -2026,7 +2026,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>0.007211321588540948</v>
+        <v>0.007211321588540886</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -2055,13 +2055,13 @@
         <v>25</v>
       </c>
       <c r="E3" t="n">
-        <v>14.20650823334482</v>
+        <v>14.20650823334481</v>
       </c>
       <c r="F3" t="n">
         <v>19.68503937007874</v>
       </c>
       <c r="G3" t="n">
-        <v>5.478531136733925</v>
+        <v>5.478531136733936</v>
       </c>
       <c r="H3" t="n">
         <v>13.7041329128455</v>
@@ -2075,7 +2075,7 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>0.09674204393942998</v>
+        <v>0.09674204393942937</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -2110,7 +2110,7 @@
         <v>22.83464566929134</v>
       </c>
       <c r="G4" t="n">
-        <v>7.774369215401114</v>
+        <v>7.774369215401119</v>
       </c>
       <c r="H4" t="n">
         <v>16.39556223010246</v>
@@ -2124,7 +2124,7 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>0.01817058965418706</v>
+        <v>0.01817058965418702</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -2153,13 +2153,13 @@
         <v>30</v>
       </c>
       <c r="E5" t="n">
-        <v>15.26187809239385</v>
+        <v>15.26187809239384</v>
       </c>
       <c r="F5" t="n">
         <v>23.62204724409449</v>
       </c>
       <c r="G5" t="n">
-        <v>8.360169151700635</v>
+        <v>8.360169151700644</v>
       </c>
       <c r="H5" t="n">
         <v>17.07730427990417</v>
@@ -2173,7 +2173,7 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0.01299428876467788</v>
+        <v>0.01299428876467781</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -2398,7 +2398,7 @@
         <v>20</v>
       </c>
       <c r="E10" t="n">
-        <v>27.65751553896241</v>
+        <v>27.6575155389624</v>
       </c>
       <c r="F10" t="n">
         <v>15.74803149606299</v>
@@ -2418,7 +2418,7 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>0.002009510472288933</v>
+        <v>0.00200951047228893</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -2447,13 +2447,13 @@
         <v>34</v>
       </c>
       <c r="E11" t="n">
-        <v>29.06894455622045</v>
+        <v>29.06894455622044</v>
       </c>
       <c r="F11" t="n">
         <v>25.37313432835821</v>
       </c>
       <c r="G11" t="n">
-        <v>-3.69581022786224</v>
+        <v>-3.695810227862228</v>
       </c>
       <c r="H11" t="n">
         <v>18.76281924434715</v>
@@ -2467,7 +2467,7 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>0.3921068605837161</v>
+        <v>0.3921068605837145</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>

</xml_diff>